<commit_message>
adds topics over time vis
</commit_message>
<xml_diff>
--- a/findings/kemal_kilicdaroglu.xlsx
+++ b/findings/kemal_kilicdaroglu.xlsx
@@ -457,48 +457,48 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>buluş, millet, oy, imza, seçim</t>
+          <t>millet, oy, buluş, sandık, seçim</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>tv, program, konuk, yayın, canlı</t>
+          <t>atatürk, önder, kemal, kutlu, gazi</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>yayın, program, canlı, konuk, sun</t>
+          <t>bayram, atatürk, türk, kutlu, mustafa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gel, bura, haydi, eşik, sev</t>
+          <t>tv, program, konuk, yayın, fox</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gel, saat, bekle, sizinle, yalnız</t>
+          <t>yayın, program, canlı, konuk, sun</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>basın, açıkla, kktc, dön, medya</t>
+          <t>sağduyu, pis, yeter, çık, allah</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -506,97 +506,97 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>basın, açıkla, medya, cemiyet, uygula</t>
+          <t>iyi, sanatçı, allah, iş, çık</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>milyar, yatırım, dolar, para, yaklaşık</t>
+          <t>basın, açıkla, kktc, dön, medya</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>milyar, yatırım, lira, dolar, kamu</t>
+          <t>basın, açıkla, medya, uygula, cemiyet</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>lig, süper, rahmetli, ateş, yanıbaş</t>
+          <t>milyar, yatırım, para, dolar, lira</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>şehit, rahmet, atatürk, an, gazi</t>
+          <t>milyar, yatırım, lira, dolar, kamu</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>deprem, depremzede, konut, bölge, hele</t>
+          <t>türkiye, türk, dostluk, israil, hemen</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>konut, deprem, depremzede, temel, hastane</t>
+          <t>türk, türkiye, milliyetçi, yüzyıl, millet</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>türkiye, dostluk, israil, türk, hemen</t>
+          <t>bura, gel, haydi, buluş, bitir</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>türk, türkiye, yüzyıl, milliyetçi, azerbaycan</t>
+          <t>gel, buluş, saat, bugün, bekle</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>engelli, aile, akademisyen, yetenek, kanun</t>
+          <t>lig, süper, rahmetli, camia, ateş</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>öğretmen, emekli, maaş, eğitim, hak</t>
+          <t>şehit, rahmet, atatürk, an, dönüm</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>acı, kayıp, rahmet, çerkes, sürgün</t>
+          <t>deprem, depremzede, konut, bölge, hele</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>acı, çerkes, sürgün, kardeş, rahmet</t>
+          <t>konut, deprem, depremzede, temel, hastane</t>
         </is>
       </c>
     </row>
@@ -611,14 +611,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>genç, telefon, internet, buluş, medya</t>
+          <t>genç, internet, buluş, telefon, medya</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>kishida, benze, üzgün, roman, başbakan</t>
+          <t>acı, kayıp, çerkes, sürgün, din</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>millet, al, saldırı, chp, insan</t>
+          <t>acı, çerkes, sürgün, kardeş, kayıp</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reduces candidate num to 2
</commit_message>
<xml_diff>
--- a/findings/kemal_kilicdaroglu.xlsx
+++ b/findings/kemal_kilicdaroglu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,197 +436,238 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Topic</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Words</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>buluş, millet, sandık, referandum, seçim</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>68</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>millet, oy, buluş, sandık, seçim</t>
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>buluş, millet, muhteşem, adana, antalya</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>72</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>buluş, millet, muhteşem, erzurum, hatay</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>atatürk, önder, kemal, kutlu, gazi</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>16</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>bayram, atatürk, türk, kutlu, mustafa</t>
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sandık, seçim, demokrasi, genç, millet</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>27</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>seçim, sandık, millet, mayıs, oy</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>tv, program, konuk, yayın, fox</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>14</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>yayın, program, canlı, konuk, sun</t>
+      <c r="A4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>tv, basın, açıkla, konuk, program</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>27</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>canlı, yayın, tv, basın, açıkla</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sağduyu, pis, yeter, çık, allah</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>rahmet, dile, allah, lig, asker</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>rahmet, atatürk, şehit, dile, allah</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gel, sev, haydi, vatan, bura</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gel, sev, haydi, vatan, bura</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>türkiye, türk, dünya, ülke, bahar</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>19</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>türkiye, yüzyıl, ülke, mayıs, millet</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>deprem, depremzede, konut, bölge, vatandaş</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>konut, deprem, temel, at, ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>13</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>para, yatırım, erdoğan, ver, ekonomist</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>para, yatırım, erdoğan, çalış, ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>teşekkür, sık, baba, kutlu, bayram</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>teşekkür, kardeş, muhteşem, güzel, istanbul</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>12</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>iyi, sanatçı, allah, iş, çık</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>basın, açıkla, kktc, dön, medya</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>12</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>basın, açıkla, medya, uygula, cemiyet</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>milyar, yatırım, para, dolar, lira</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>11</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>milyar, yatırım, lira, dolar, kamu</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>türkiye, türk, dostluk, israil, hemen</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>türk, türkiye, milliyetçi, yüzyıl, millet</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>bura, gel, haydi, buluş, bitir</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>gel, buluş, saat, bugün, bekle</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>lig, süper, rahmetli, camia, ateş</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>engelli, akademisyen, yetenek, öğretmen, iyi</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>öğretmen, ata, eğitim, engelli, okul</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>8</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>şehit, rahmet, atatürk, an, dönüm</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>deprem, depremzede, konut, bölge, hele</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>konut, deprem, depremzede, temel, hastane</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>genç, demirel, ak, salon, partili</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>6</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>genç, internet, buluş, telefon, medya</t>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>milyar, yatırım, yaklaşık, tl, kul</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>milyar, yatırım, lira, kamu, dolar</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>acı, kayıp, çerkes, sürgün, din</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>acı, çerkes, sürgün, kardeş, kayıp</t>
+      <c r="A13" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>karınca, atom, azim, enerji, kazan</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nükleer, santral, enerji, üretim, ülke</t>
         </is>
       </c>
     </row>

</xml_diff>